<commit_message>
Correction to Data in several tests. Added comments to Linear Tests. Added .gitignore
</commit_message>
<xml_diff>
--- a/resources/Data.xlsx
+++ b/resources/Data.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{ADA008A5-00D2-4E3B-BAFA-7D74C6C271B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\testautomation\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C74562D-74AA-4066-82A8-1D60486B5574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="29070" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -389,7 +393,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" sqref="A5:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +402,7 @@
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -412,7 +416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -426,7 +430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -440,7 +444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>

</xml_diff>